<commit_message>
Cambiando la vista Movimientos
Cambiando la apariencia de la vista Movimientos

Se realizó nuevas consultas y se agregó una nueva vista a la plantilla Movimientos y se utilizó un nuevo plugin de JQuery llamabdo boostrap-select compatible con la versión 3.1.1
</commit_message>
<xml_diff>
--- a/docs/backup/cuenta_12196038826.xlsx
+++ b/docs/backup/cuenta_12196038826.xlsx
@@ -14,15 +14,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>C</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>509.04</t>
+  </si>
+  <si>
+    <t>CRE</t>
+  </si>
+  <si>
+    <t>0000005690</t>
+  </si>
+  <si>
+    <t>AGENCIA EXPRESS GIRON</t>
+  </si>
+  <si>
+    <t>RETI</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>0000007767</t>
+  </si>
+  <si>
+    <t>9.04</t>
   </si>
 </sst>
 </file>
@@ -369,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H1" sqref="H1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,29 +400,56 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>41796</v>
+        <v>41802</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="str">
+        <f ca="1">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",F1,", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-06-12'), 'mo_concepto' =&gt; 'RETI', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0000007767', 'mo_oficina' =&gt; 'AGENCIA EXPRESS GIRON', 'mo_monto' =&gt; 9.04, 'mo_saldo' =&gt; 9.04, 'mo_fecha_crea' =&gt; new \DateTime('2014-06-17 21:30:6'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>41789</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" t="str">
-        <f t="shared" ref="H1" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",F1,", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-06-06'), 'mo_concepto' =&gt; '-', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '-', 'mo_oficina' =&gt; '-', 'mo_monto' =&gt; 509.04, 'mo_saldo' =&gt; 509.04, 'mo_fecha_crea' =&gt; new \DateTime('2014-06-07 15:28:28'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+      <c r="H2" t="str">
+        <f ca="1">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A2,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B2,"', 'mo_tipo' =&gt; '",C2,"', 'mo_documento' =&gt; '",D2,"', 'mo_oficina' =&gt; '",E2,"', 'mo_monto' =&gt; ",F2,", 'mo_saldo' =&gt; ",G2,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-05-30'), 'mo_concepto' =&gt; 'CRE', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0000005690', 'mo_oficina' =&gt; 'AGENCIA EXPRESS GIRON', 'mo_monto' =&gt; 509.04, 'mo_saldo' =&gt; 509.04, 'mo_fecha_crea' =&gt; new \DateTime('2014-06-17 21:30:6'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizando los movimeintos de las cuentas
Se añade también un archivo de parametros de acceso al bdd para que sea despues un ejemplo de como
trabajar con el. El archivo parameters.yml fue eliminado para que conste en el .gitignore
</commit_message>
<xml_diff>
--- a/docs/backup/cuenta_12196038826.xlsx
+++ b/docs/backup/cuenta_12196038826.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>C</t>
   </si>
@@ -22,25 +22,73 @@
     <t>509.04</t>
   </si>
   <si>
-    <t>CRE</t>
-  </si>
-  <si>
-    <t>0000005690</t>
-  </si>
-  <si>
-    <t>AGENCIA EXPRESS GIRON</t>
-  </si>
-  <si>
-    <t>RETI</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
-    <t>0000007767</t>
-  </si>
-  <si>
     <t>9.04</t>
+  </si>
+  <si>
+    <t>ROL DE PAGOS</t>
+  </si>
+  <si>
+    <t>0197325546</t>
+  </si>
+  <si>
+    <t>MATRIZ - QUITO</t>
+  </si>
+  <si>
+    <t>RETIRO CON LIBRETA</t>
+  </si>
+  <si>
+    <t>0031789350</t>
+  </si>
+  <si>
+    <t>AG. PDBCO EXPRESS EL GIRÓN QUI</t>
+  </si>
+  <si>
+    <t>1175.18</t>
+  </si>
+  <si>
+    <t>1184.22</t>
+  </si>
+  <si>
+    <t>CAPITALIZACION DE INTERESES EN CUENTA</t>
+  </si>
+  <si>
+    <t>0.08</t>
+  </si>
+  <si>
+    <t>1184.30</t>
+  </si>
+  <si>
+    <t>AG. PDBCO EXPRESS MEGAMAXI UIO</t>
+  </si>
+  <si>
+    <t>1000.00</t>
+  </si>
+  <si>
+    <t>184.30</t>
+  </si>
+  <si>
+    <t>RETIROS ATM CLIENTES PRODUBANCO</t>
+  </si>
+  <si>
+    <t>180.00</t>
+  </si>
+  <si>
+    <t>4.30</t>
+  </si>
+  <si>
+    <t>0199880577</t>
+  </si>
+  <si>
+    <t>0020140630</t>
+  </si>
+  <si>
+    <t>0028525948</t>
+  </si>
+  <si>
+    <t>9382000143</t>
   </si>
 </sst>
 </file>
@@ -387,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H2"/>
+      <selection activeCell="H6" sqref="H1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,56 +448,164 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>41802</v>
+        <v>41822</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="H1" t="str">
-        <f ca="1">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",F1,", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-06-12'), 'mo_concepto' =&gt; 'RETI', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0000007767', 'mo_oficina' =&gt; 'AGENCIA EXPRESS GIRON', 'mo_monto' =&gt; 9.04, 'mo_saldo' =&gt; 9.04, 'mo_fecha_crea' =&gt; new \DateTime('2014-06-17 21:30:6'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <f t="shared" ref="H1:H4" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",F1,", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-07-02'), 'mo_concepto' =&gt; 'RETIROS ATM CLIENTES PRODUBANCO', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '9382000143', 'mo_oficina' =&gt; 'AG. PDBCO EXPRESS MEGAMAXI UIO', 'mo_monto' =&gt; 180.00, 'mo_saldo' =&gt; 4.30, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-03 14:52:20'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
+        <v>41822</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-07-02'), 'mo_concepto' =&gt; 'RETIRO CON LIBRETA', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0028525948', 'mo_oficina' =&gt; 'AG. PDBCO EXPRESS MEGAMAXI UIO', 'mo_monto' =&gt; 1000.00, 'mo_saldo' =&gt; 184.30, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-03 14:52:20'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>41820</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-06-30'), 'mo_concepto' =&gt; 'CAPITALIZACION DE INTERESES EN CUENTA', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0020140630', 'mo_oficina' =&gt; 'MATRIZ - QUITO', 'mo_monto' =&gt; 0.08, 'mo_saldo' =&gt; 1184.30, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-03 14:52:20'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>41820</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-06-30'), 'mo_concepto' =&gt; 'ROL DE PAGOS', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0199880577', 'mo_oficina' =&gt; 'MATRIZ - QUITO', 'mo_monto' =&gt; 1175.18, 'mo_saldo' =&gt; 1184.22, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-03 14:52:20'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>41802</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" t="str">
+        <f ca="1">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A5,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B5,"', 'mo_tipo' =&gt; '",C5,"', 'mo_documento' =&gt; '",D5,"', 'mo_oficina' =&gt; '",E5,"', 'mo_monto' =&gt; ",F5,", 'mo_saldo' =&gt; ",G5,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-06-12'), 'mo_concepto' =&gt; 'RETIRO CON LIBRETA', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0031789350', 'mo_oficina' =&gt; 'AG. PDBCO EXPRESS EL GIRÓN QUI', 'mo_monto' =&gt; 9.04, 'mo_saldo' =&gt; 9.04, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-03 14:52:20'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>41789</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H2" t="str">
-        <f ca="1">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A2,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B2,"', 'mo_tipo' =&gt; '",C2,"', 'mo_documento' =&gt; '",D2,"', 'mo_oficina' =&gt; '",E2,"', 'mo_monto' =&gt; ",F2,", 'mo_saldo' =&gt; ",G2,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-05-30'), 'mo_concepto' =&gt; 'CRE', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0000005690', 'mo_oficina' =&gt; 'AGENCIA EXPRESS GIRON', 'mo_monto' =&gt; 509.04, 'mo_saldo' =&gt; 509.04, 'mo_fecha_crea' =&gt; new \DateTime('2014-06-17 21:30:6'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+      <c r="H6" t="str">
+        <f ca="1">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A6,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B6,"', 'mo_tipo' =&gt; '",C6,"', 'mo_documento' =&gt; '",D6,"', 'mo_oficina' =&gt; '",E6,"', 'mo_monto' =&gt; ",F6,", 'mo_saldo' =&gt; ",G6,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-05-30'), 'mo_concepto' =&gt; 'ROL DE PAGOS', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0197325546', 'mo_oficina' =&gt; 'MATRIZ - QUITO', 'mo_monto' =&gt; 509.04, 'mo_saldo' =&gt; 509.04, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-03 14:52:20'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizando modelo de base de datos y fixtures
Actualizando el modelo d bdd y recarga de Movimientos en el fixtures

Se modificó el campo  mo_documento aumentando un poco mas el string para numeros de documentos
grandes como es el caso de Produbanco a lavez que se actualizó el las clases que recargan datos con
el método fixtures. Ademas se reubicó una clase repositorio llamada Hijos.
</commit_message>
<xml_diff>
--- a/docs/backup/cuenta_12196038826.xlsx
+++ b/docs/backup/cuenta_12196038826.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>C</t>
   </si>
@@ -89,6 +89,21 @@
   </si>
   <si>
     <t>9382000143</t>
+  </si>
+  <si>
+    <t>PAGO MOVISTAR</t>
+  </si>
+  <si>
+    <t>641925020506</t>
+  </si>
+  <si>
+    <t>500.00</t>
+  </si>
+  <si>
+    <t>3.00</t>
+  </si>
+  <si>
+    <t>1.30</t>
   </si>
 </sst>
 </file>
@@ -435,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H1:H6"/>
+      <selection activeCell="H7" sqref="H1:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,29 +463,29 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>41822</v>
+        <v>41834</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="H1" t="str">
-        <f t="shared" ref="H1:H4" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",F1,", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-07-02'), 'mo_concepto' =&gt; 'RETIROS ATM CLIENTES PRODUBANCO', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '9382000143', 'mo_oficina' =&gt; 'AG. PDBCO EXPRESS MEGAMAXI UIO', 'mo_monto' =&gt; 180.00, 'mo_saldo' =&gt; 4.30, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-03 14:52:20'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <f t="shared" ref="H1:H5" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",F1,", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-07-14'), 'mo_concepto' =&gt; 'PAGO MOVISTAR', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '641925020506', 'mo_oficina' =&gt; 'MATRIZ - QUITO', 'mo_monto' =&gt; 3.00, 'mo_saldo' =&gt; 1.30, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-15 20:21:8'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -478,53 +493,53 @@
         <v>41822</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-07-02'), 'mo_concepto' =&gt; 'RETIRO CON LIBRETA', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0028525948', 'mo_oficina' =&gt; 'AG. PDBCO EXPRESS MEGAMAXI UIO', 'mo_monto' =&gt; 1000.00, 'mo_saldo' =&gt; 184.30, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-03 14:52:20'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-07-02'), 'mo_concepto' =&gt; 'RETIROS ATM CLIENTES PRODUBANCO', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '9382000143', 'mo_oficina' =&gt; 'AG. PDBCO EXPRESS MEGAMAXI UIO', 'mo_monto' =&gt; 180.00, 'mo_saldo' =&gt; 4.30, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-15 20:21:8'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>41820</v>
+        <v>41822</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-06-30'), 'mo_concepto' =&gt; 'CAPITALIZACION DE INTERESES EN CUENTA', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0020140630', 'mo_oficina' =&gt; 'MATRIZ - QUITO', 'mo_monto' =&gt; 0.08, 'mo_saldo' =&gt; 1184.30, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-03 14:52:20'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-07-02'), 'mo_concepto' =&gt; 'RETIRO CON LIBRETA', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0028525948', 'mo_oficina' =&gt; 'AG. PDBCO EXPRESS MEGAMAXI UIO', 'mo_monto' =&gt; 1000.00, 'mo_saldo' =&gt; 184.30, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-15 20:21:8'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -532,80 +547,107 @@
         <v>41820</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-06-30'), 'mo_concepto' =&gt; 'ROL DE PAGOS', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0199880577', 'mo_oficina' =&gt; 'MATRIZ - QUITO', 'mo_monto' =&gt; 1175.18, 'mo_saldo' =&gt; 1184.22, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-03 14:52:20'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-06-30'), 'mo_concepto' =&gt; 'CAPITALIZACION DE INTERESES EN CUENTA', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0020140630', 'mo_oficina' =&gt; 'MATRIZ - QUITO', 'mo_monto' =&gt; 0.08, 'mo_saldo' =&gt; 1184.30, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-15 20:21:8'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>41802</v>
+        <v>41820</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H5" t="str">
-        <f ca="1">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A5,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B5,"', 'mo_tipo' =&gt; '",C5,"', 'mo_documento' =&gt; '",D5,"', 'mo_oficina' =&gt; '",E5,"', 'mo_monto' =&gt; ",F5,", 'mo_saldo' =&gt; ",G5,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-06-12'), 'mo_concepto' =&gt; 'RETIRO CON LIBRETA', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0031789350', 'mo_oficina' =&gt; 'AG. PDBCO EXPRESS EL GIRÓN QUI', 'mo_monto' =&gt; 9.04, 'mo_saldo' =&gt; 9.04, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-03 14:52:20'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-06-30'), 'mo_concepto' =&gt; 'ROL DE PAGOS', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0199880577', 'mo_oficina' =&gt; 'MATRIZ - QUITO', 'mo_monto' =&gt; 1175.18, 'mo_saldo' =&gt; 1184.22, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-15 20:21:8'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>41789</v>
+        <v>41802</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>1</v>
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>3</v>
       </c>
       <c r="H6" t="str">
         <f ca="1">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A6,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B6,"', 'mo_tipo' =&gt; '",C6,"', 'mo_documento' =&gt; '",D6,"', 'mo_oficina' =&gt; '",E6,"', 'mo_monto' =&gt; ",F6,", 'mo_saldo' =&gt; ",G6,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-05-30'), 'mo_concepto' =&gt; 'ROL DE PAGOS', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0197325546', 'mo_oficina' =&gt; 'MATRIZ - QUITO', 'mo_monto' =&gt; 509.04, 'mo_saldo' =&gt; 509.04, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-03 14:52:20'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-06-12'), 'mo_concepto' =&gt; 'RETIRO CON LIBRETA', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0031789350', 'mo_oficina' =&gt; 'AG. PDBCO EXPRESS EL GIRÓN QUI', 'mo_monto' =&gt; 500.00, 'mo_saldo' =&gt; 9.04, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-15 20:21:8'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>41789</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" t="str">
+        <f ca="1">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A7,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B7,"', 'mo_tipo' =&gt; '",C7,"', 'mo_documento' =&gt; '",D7,"', 'mo_oficina' =&gt; '",E7,"', 'mo_monto' =&gt; ",F7,", 'mo_saldo' =&gt; ",G7,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-05-30'), 'mo_concepto' =&gt; 'ROL DE PAGOS', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0197325546', 'mo_oficina' =&gt; 'MATRIZ - QUITO', 'mo_monto' =&gt; 509.04, 'mo_saldo' =&gt; 509.04, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-15 20:21:8'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactorizando la clase LoadMovimientos
Refactorizando la clase LoadMovimientos para la carga de datos en el Fixtures

Se mejoró el código en la clase LoadMovimientos para la carga de datos de los movimientos
bancarios obteniendo mejor rendimiento y entendimiento.
</commit_message>
<xml_diff>
--- a/docs/backup/cuenta_12196038826.xlsx
+++ b/docs/backup/cuenta_12196038826.xlsx
@@ -31,18 +31,12 @@
     <t>ROL DE PAGOS</t>
   </si>
   <si>
-    <t>0197325546</t>
-  </si>
-  <si>
     <t>MATRIZ - QUITO</t>
   </si>
   <si>
     <t>RETIRO CON LIBRETA</t>
   </si>
   <si>
-    <t>0031789350</t>
-  </si>
-  <si>
     <t>AG. PDBCO EXPRESS EL GIRÓN QUI</t>
   </si>
   <si>
@@ -79,18 +73,6 @@
     <t>4.30</t>
   </si>
   <si>
-    <t>0199880577</t>
-  </si>
-  <si>
-    <t>0020140630</t>
-  </si>
-  <si>
-    <t>0028525948</t>
-  </si>
-  <si>
-    <t>9382000143</t>
-  </si>
-  <si>
     <t>PAGO MOVISTAR</t>
   </si>
   <si>
@@ -104,6 +86,24 @@
   </si>
   <si>
     <t>1.30</t>
+  </si>
+  <si>
+    <t>009382000143</t>
+  </si>
+  <si>
+    <t>000028525948</t>
+  </si>
+  <si>
+    <t>000020140630</t>
+  </si>
+  <si>
+    <t>000199880577</t>
+  </si>
+  <si>
+    <t>000031789350</t>
+  </si>
+  <si>
+    <t>000197325546</t>
   </si>
 </sst>
 </file>
@@ -458,7 +458,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="11.7109375" customWidth="1"/>
+    <col min="1" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -466,26 +468,26 @@
         <v>41834</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H1" t="str">
-        <f t="shared" ref="H1:H5" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",F1,", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-07-14'), 'mo_concepto' =&gt; 'PAGO MOVISTAR', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '641925020506', 'mo_oficina' =&gt; 'MATRIZ - QUITO', 'mo_monto' =&gt; 3.00, 'mo_saldo' =&gt; 1.30, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-15 20:21:8'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <f t="shared" ref="H1:H6" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",F1,", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-07-14'), 'mo_concepto' =&gt; 'PAGO MOVISTAR', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '641925020506', 'mo_oficina' =&gt; 'MATRIZ - QUITO', 'mo_monto' =&gt; 3.00, 'mo_saldo' =&gt; 1.30, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-15 21:57:11'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -493,7 +495,7 @@
         <v>41822</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -502,17 +504,17 @@
         <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H2" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-07-02'), 'mo_concepto' =&gt; 'RETIROS ATM CLIENTES PRODUBANCO', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '9382000143', 'mo_oficina' =&gt; 'AG. PDBCO EXPRESS MEGAMAXI UIO', 'mo_monto' =&gt; 180.00, 'mo_saldo' =&gt; 4.30, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-15 20:21:8'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-07-02'), 'mo_concepto' =&gt; 'RETIROS ATM CLIENTES PRODUBANCO', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '009382000143', 'mo_oficina' =&gt; 'AG. PDBCO EXPRESS MEGAMAXI UIO', 'mo_monto' =&gt; 180.00, 'mo_saldo' =&gt; 4.30, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-15 21:57:11'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -520,26 +522,26 @@
         <v>41822</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-07-02'), 'mo_concepto' =&gt; 'RETIRO CON LIBRETA', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0028525948', 'mo_oficina' =&gt; 'AG. PDBCO EXPRESS MEGAMAXI UIO', 'mo_monto' =&gt; 1000.00, 'mo_saldo' =&gt; 184.30, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-15 20:21:8'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-07-02'), 'mo_concepto' =&gt; 'RETIRO CON LIBRETA', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '000028525948', 'mo_oficina' =&gt; 'AG. PDBCO EXPRESS MEGAMAXI UIO', 'mo_monto' =&gt; 1000.00, 'mo_saldo' =&gt; 184.30, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-15 21:57:11'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -547,26 +549,26 @@
         <v>41820</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-06-30'), 'mo_concepto' =&gt; 'CAPITALIZACION DE INTERESES EN CUENTA', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0020140630', 'mo_oficina' =&gt; 'MATRIZ - QUITO', 'mo_monto' =&gt; 0.08, 'mo_saldo' =&gt; 1184.30, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-15 20:21:8'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-06-30'), 'mo_concepto' =&gt; 'CAPITALIZACION DE INTERESES EN CUENTA', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '000020140630', 'mo_oficina' =&gt; 'MATRIZ - QUITO', 'mo_monto' =&gt; 0.08, 'mo_saldo' =&gt; 1184.30, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-15 21:57:11'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -580,20 +582,20 @@
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-06-30'), 'mo_concepto' =&gt; 'ROL DE PAGOS', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0199880577', 'mo_oficina' =&gt; 'MATRIZ - QUITO', 'mo_monto' =&gt; 1175.18, 'mo_saldo' =&gt; 1184.22, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-15 20:21:8'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-06-30'), 'mo_concepto' =&gt; 'ROL DE PAGOS', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '000199880577', 'mo_oficina' =&gt; 'MATRIZ - QUITO', 'mo_monto' =&gt; 1175.18, 'mo_saldo' =&gt; 1184.22, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-15 21:57:11'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -601,26 +603,26 @@
         <v>41802</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
         <v>3</v>
       </c>
       <c r="H6" t="str">
-        <f ca="1">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A6,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B6,"', 'mo_tipo' =&gt; '",C6,"', 'mo_documento' =&gt; '",D6,"', 'mo_oficina' =&gt; '",E6,"', 'mo_monto' =&gt; ",F6,", 'mo_saldo' =&gt; ",G6,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-06-12'), 'mo_concepto' =&gt; 'RETIRO CON LIBRETA', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '0031789350', 'mo_oficina' =&gt; 'AG. PDBCO EXPRESS EL GIRÓN QUI', 'mo_monto' =&gt; 500.00, 'mo_saldo' =&gt; 9.04, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-15 20:21:8'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-06-12'), 'mo_concepto' =&gt; 'RETIRO CON LIBRETA', 'mo_tipo' =&gt; 'D', 'mo_documento' =&gt; '000031789350', 'mo_oficina' =&gt; 'AG. PDBCO EXPRESS EL GIRÓN QUI', 'mo_monto' =&gt; 500.00, 'mo_saldo' =&gt; 9.04, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-15 21:57:11'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -634,10 +636,10 @@
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
         <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>1</v>
@@ -647,7 +649,7 @@
       </c>
       <c r="H7" t="str">
         <f ca="1">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A7,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B7,"', 'mo_tipo' =&gt; '",C7,"', 'mo_documento' =&gt; '",D7,"', 'mo_oficina' =&gt; '",E7,"', 'mo_monto' =&gt; ",F7,", 'mo_saldo' =&gt; ",G7,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-05-30'), 'mo_concepto' =&gt; 'ROL DE PAGOS', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0197325546', 'mo_oficina' =&gt; 'MATRIZ - QUITO', 'mo_monto' =&gt; 509.04, 'mo_saldo' =&gt; 509.04, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-15 20:21:8'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-05-30'), 'mo_concepto' =&gt; 'ROL DE PAGOS', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '000197325546', 'mo_oficina' =&gt; 'MATRIZ - QUITO', 'mo_monto' =&gt; 509.04, 'mo_saldo' =&gt; 509.04, 'mo_fecha_crea' =&gt; new \DateTime('2014-07-15 21:57:11'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_fecha_borrado' =&gt; NULL, 'mo_quien_borra' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
   </sheetData>

</xml_diff>